<commit_message>
Update stats for 2025-07
</commit_message>
<xml_diff>
--- a/iserv_stats.xlsx
+++ b/iserv_stats.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,6 +463,21 @@
           <t>users_per_school</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>yoy_schools</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>yoy_authorities</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>yoy_users</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
@@ -480,6 +495,9 @@
       <c r="E2" t="n">
         <v>677.645789839944</v>
       </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
@@ -497,6 +515,9 @@
       <c r="E3" t="n">
         <v>680.28118466899</v>
       </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
@@ -514,6 +535,9 @@
       <c r="E4" t="n">
         <v>684.802679658953</v>
       </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
@@ -531,6 +555,9 @@
       <c r="E5" t="n">
         <v>742.137113764045</v>
       </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
@@ -548,6 +575,9 @@
       <c r="E6" t="n">
         <v>750.380777310924</v>
       </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
@@ -565,6 +595,9 @@
       <c r="E7" t="n">
         <v>759.158481365378</v>
       </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
@@ -582,6 +615,9 @@
       <c r="E8" t="n">
         <v>763.633269994818</v>
       </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
@@ -599,6 +635,9 @@
       <c r="E9" t="n">
         <v>760.4533935080721</v>
       </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
@@ -616,6 +655,9 @@
       <c r="E10" t="n">
         <v>791.592356687898</v>
       </c>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
@@ -633,6 +675,9 @@
       <c r="E11" t="n">
         <v>800.774365133837</v>
       </c>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
@@ -650,6 +695,9 @@
       <c r="E12" t="n">
         <v>804.73440163655</v>
       </c>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
@@ -667,6 +715,9 @@
       <c r="E13" t="n">
         <v>810.532337463928</v>
       </c>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
@@ -684,6 +735,15 @@
       <c r="E14" t="n">
         <v>811.5452087206349</v>
       </c>
+      <c r="F14" t="n">
+        <v>2.940153096729303</v>
+      </c>
+      <c r="G14" t="n">
+        <v>5.961754780652417</v>
+      </c>
+      <c r="H14" t="n">
+        <v>23.28061250163025</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
@@ -701,6 +761,15 @@
       <c r="E15" t="n">
         <v>819.412941176471</v>
       </c>
+      <c r="F15" t="n">
+        <v>3.658536585365857</v>
+      </c>
+      <c r="G15" t="n">
+        <v>6.764374295377684</v>
+      </c>
+      <c r="H15" t="n">
+        <v>24.85887932178075</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
@@ -718,6 +787,15 @@
       <c r="E16" t="n">
         <v>823.161204013378</v>
       </c>
+      <c r="F16" t="n">
+        <v>4.054289194362282</v>
+      </c>
+      <c r="G16" t="n">
+        <v>6.877113866967299</v>
+      </c>
+      <c r="H16" t="n">
+        <v>25.07756835683654</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
@@ -735,6 +813,15 @@
       <c r="E17" t="n">
         <v>833.321558872305</v>
       </c>
+      <c r="F17" t="n">
+        <v>5.86376404494382</v>
+      </c>
+      <c r="G17" t="n">
+        <v>3.205128205128216</v>
+      </c>
+      <c r="H17" t="n">
+        <v>18.87096770378025</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
@@ -752,6 +839,15 @@
       <c r="E18" t="n">
         <v>837.5488448844879</v>
       </c>
+      <c r="F18" t="n">
+        <v>6.092436974789917</v>
+      </c>
+      <c r="G18" t="n">
+        <v>3.311965811965822</v>
+      </c>
+      <c r="H18" t="n">
+        <v>18.41667687390272</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
@@ -769,6 +865,15 @@
       <c r="E19" t="n">
         <v>889.72649852604</v>
       </c>
+      <c r="F19" t="n">
+        <v>6.339254615116685</v>
+      </c>
+      <c r="G19" t="n">
+        <v>3.201707577374591</v>
+      </c>
+      <c r="H19" t="n">
+        <v>24.62859203576528</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
@@ -781,10 +886,19 @@
         <v>975</v>
       </c>
       <c r="D20" t="n">
-        <v>5551601</v>
+        <v>5551604</v>
       </c>
       <c r="E20" t="n">
-        <v>903.1399056450301</v>
+        <v>903.1403936879778</v>
+      </c>
+      <c r="F20" t="n">
+        <v>6.184142338918641</v>
+      </c>
+      <c r="G20" t="n">
+        <v>3.503184713375807</v>
+      </c>
+      <c r="H20" t="n">
+        <v>25.58277891171774</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update stats for 2025-08
</commit_message>
<xml_diff>
--- a/iserv_stats.xlsx
+++ b/iserv_stats.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -901,6 +901,32 @@
         <v>26.25489376843753</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>45870</v>
+      </c>
+      <c r="B21" t="n">
+        <v>6208</v>
+      </c>
+      <c r="C21" t="n">
+        <v>980</v>
+      </c>
+      <c r="D21" t="n">
+        <v>5584698</v>
+      </c>
+      <c r="E21" t="n">
+        <v>899.5969716494845</v>
+      </c>
+      <c r="F21" t="n">
+        <v>7.759069605971192</v>
+      </c>
+      <c r="G21" t="n">
+        <v>3.375527426160341</v>
+      </c>
+      <c r="H21" t="n">
+        <v>27.4762313020946</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update stats for 2025-09
</commit_message>
<xml_diff>
--- a/iserv_stats.xlsx
+++ b/iserv_stats.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -927,6 +927,32 @@
         <v>29.75572544175129</v>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>45901</v>
+      </c>
+      <c r="B22" t="n">
+        <v>6269</v>
+      </c>
+      <c r="C22" t="n">
+        <v>992</v>
+      </c>
+      <c r="D22" t="n">
+        <v>5696013</v>
+      </c>
+      <c r="E22" t="n">
+        <v>908.5999361939703</v>
+      </c>
+      <c r="F22" t="n">
+        <v>7.918746772249952</v>
+      </c>
+      <c r="G22" t="n">
+        <v>3.765690376569042</v>
+      </c>
+      <c r="H22" t="n">
+        <v>23.87053210274967</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update stats for 2025-10
</commit_message>
<xml_diff>
--- a/iserv_stats.xlsx
+++ b/iserv_stats.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -953,6 +953,32 @@
         <v>27.58320357692743</v>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
+        <v>45931</v>
+      </c>
+      <c r="B23" t="n">
+        <v>6303</v>
+      </c>
+      <c r="C23" t="n">
+        <v>996</v>
+      </c>
+      <c r="D23" t="n">
+        <v>5866825</v>
+      </c>
+      <c r="E23" t="n">
+        <v>930.798825955894</v>
+      </c>
+      <c r="F23" t="n">
+        <v>8.150308853809207</v>
+      </c>
+      <c r="G23" t="n">
+        <v>3.642039542143594</v>
+      </c>
+      <c r="H23" t="n">
+        <v>25.71104282423948</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update stats for 2025-11
</commit_message>
<xml_diff>
--- a/iserv_stats.xlsx
+++ b/iserv_stats.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -979,6 +979,32 @@
         <v>26.96508377164948</v>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
+        <v>45962</v>
+      </c>
+      <c r="B24" t="n">
+        <v>6326</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1001</v>
+      </c>
+      <c r="D24" t="n">
+        <v>5923299</v>
+      </c>
+      <c r="E24" t="n">
+        <v>936.3419222257351</v>
+      </c>
+      <c r="F24" t="n">
+        <v>7.841800204568705</v>
+      </c>
+      <c r="G24" t="n">
+        <v>3.730569948186524</v>
+      </c>
+      <c r="H24" t="n">
+        <v>25.47841659866643</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update stats for 2025-12
</commit_message>
<xml_diff>
--- a/iserv_stats.xlsx
+++ b/iserv_stats.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1005,6 +1005,32 @@
         <v>26.84566616079578</v>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" s="2" t="n">
+        <v>45992</v>
+      </c>
+      <c r="B25" t="n">
+        <v>6435</v>
+      </c>
+      <c r="C25" t="n">
+        <v>1003</v>
+      </c>
+      <c r="D25" t="n">
+        <v>5994969</v>
+      </c>
+      <c r="E25" t="n">
+        <v>931.6191142191142</v>
+      </c>
+      <c r="F25" t="n">
+        <v>9.234425394669831</v>
+      </c>
+      <c r="G25" t="n">
+        <v>6.929637526652455</v>
+      </c>
+      <c r="H25" t="n">
+        <v>25.55313825828101</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update stats for 2026-01
</commit_message>
<xml_diff>
--- a/iserv_stats.xlsx
+++ b/iserv_stats.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1031,6 +1031,32 @@
         <v>26.56682540127995</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
+        <v>46023</v>
+      </c>
+      <c r="B26" t="n">
+        <v>6479</v>
+      </c>
+      <c r="C26" t="n">
+        <v>1010</v>
+      </c>
+      <c r="D26" t="n">
+        <v>6043294</v>
+      </c>
+      <c r="E26" t="n">
+        <v>932.7510418274425</v>
+      </c>
+      <c r="F26" t="n">
+        <v>9.498056447524084</v>
+      </c>
+      <c r="G26" t="n">
+        <v>7.218683651804669</v>
+      </c>
+      <c r="H26" t="n">
+        <v>25.8518011467513</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update stats for 2026-02
</commit_message>
<xml_diff>
--- a/iserv_stats.xlsx
+++ b/iserv_stats.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1045,6 +1045,32 @@
         <v>26.9092755324805</v>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>46054</v>
+      </c>
+      <c r="B27" t="n">
+        <v>6532</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1016</v>
+      </c>
+      <c r="D27" t="n">
+        <v>6092997</v>
+      </c>
+      <c r="E27" t="n">
+        <v>932.791947336191</v>
+      </c>
+      <c r="F27" t="n">
+        <v>9.781512605042009</v>
+      </c>
+      <c r="G27" t="n">
+        <v>7.286166842661035</v>
+      </c>
+      <c r="H27" t="n">
+        <v>24.97155680424621</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>